<commit_message>
Evaluation updated in doc and xlsx
</commit_message>
<xml_diff>
--- a/Demo/evaluation/eval_results calculos.xlsx
+++ b/Demo/evaluation/eval_results calculos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ainhoaarruabarrenaortiz/Documents/Master/PBL/pbl_glioblastoma/Demo/evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0985C143-EA67-8849-AC62-154FB9387226}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B47375BA-B37F-4C42-BA81-6EF4416FCF05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11600" yWindow="500" windowWidth="14000" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -92,7 +92,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -125,7 +125,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -431,7 +431,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -444,16 +444,16 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>0.86219944748010846</v>
+        <v>0.86219900000000005</v>
       </c>
       <c r="C1">
-        <v>0.32182802164762481</v>
+        <v>0.321828</v>
       </c>
       <c r="D1">
-        <v>0.13780055251989159</v>
+        <v>0.13780100000000001</v>
       </c>
       <c r="E1">
-        <v>0.65227808259458664</v>
+        <v>0.65227800000000002</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -461,16 +461,16 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.85189729595551178</v>
+        <v>0.85189700000000002</v>
       </c>
       <c r="C2">
-        <v>0.3646020234935835</v>
+        <v>0.36460199999999998</v>
       </c>
       <c r="D2">
-        <v>0.14810270404448819</v>
+        <v>0.14810300000000001</v>
       </c>
       <c r="E2">
-        <v>0.62428259762837546</v>
+        <v>0.62428300000000003</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -478,16 +478,16 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.91935527950571705</v>
+        <v>0.91935500000000003</v>
       </c>
       <c r="C3">
-        <v>0.1936610613459917</v>
+        <v>0.193661</v>
       </c>
       <c r="D3">
-        <v>8.0644720494282909E-2</v>
+        <v>8.0644999999999994E-2</v>
       </c>
       <c r="E3">
-        <v>0.77019793078366572</v>
+        <v>0.77019800000000005</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -495,16 +495,16 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.96246102743556317</v>
+        <v>0.96246100000000001</v>
       </c>
       <c r="C4">
-        <v>0.2338914958918662</v>
+        <v>0.23389099999999999</v>
       </c>
       <c r="D4">
-        <v>3.7538972564436821E-2</v>
+        <v>3.7539000000000003E-2</v>
       </c>
       <c r="E4">
-        <v>0.78002079651249157</v>
+        <v>0.78002099999999996</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -512,16 +512,16 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>0.87855540109481267</v>
+        <v>0.87855499999999997</v>
       </c>
       <c r="C5">
-        <v>0.38113380594475182</v>
+        <v>0.38113399999999997</v>
       </c>
       <c r="D5">
-        <v>0.1214445989051874</v>
+        <v>0.121445</v>
       </c>
       <c r="E5">
-        <v>0.6361117201774994</v>
+        <v>0.63611200000000001</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -529,16 +529,16 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>0.91689501527733341</v>
+        <v>0.91689500000000002</v>
       </c>
       <c r="C6">
-        <v>0.37417551082859252</v>
+        <v>0.37417600000000001</v>
       </c>
       <c r="D6">
-        <v>8.3104984722666558E-2</v>
+        <v>8.3104999999999998E-2</v>
       </c>
       <c r="E6">
-        <v>0.66723283019682789</v>
+        <v>0.66723299999999997</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -546,16 +546,16 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>0.89151543507220854</v>
+        <v>0.89151499999999995</v>
       </c>
       <c r="C7">
-        <v>0.54196302220419379</v>
+        <v>0.54196299999999997</v>
       </c>
       <c r="D7">
-        <v>0.1084845649277914</v>
+        <v>0.108485</v>
       </c>
       <c r="E7">
-        <v>0.57816914039729161</v>
+        <v>0.57816900000000004</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -563,16 +563,16 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>0.95064923706157944</v>
+        <v>0.95064899999999997</v>
       </c>
       <c r="C8">
-        <v>0.63086301402968892</v>
+        <v>0.63086299999999995</v>
       </c>
       <c r="D8">
-        <v>4.9350762938420577E-2</v>
+        <v>4.9350999999999999E-2</v>
       </c>
       <c r="E8">
-        <v>0.58291176443607384</v>
+        <v>0.58291199999999999</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -580,16 +580,16 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>0.86045196218385545</v>
+        <v>0.86045199999999999</v>
       </c>
       <c r="C9">
-        <v>0.35381258922078268</v>
+        <v>0.35381299999999999</v>
       </c>
       <c r="D9">
-        <v>0.13954803781614461</v>
+        <v>0.13954800000000001</v>
       </c>
       <c r="E9">
-        <v>0.63557686568648908</v>
+        <v>0.63557699999999995</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -597,16 +597,16 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>0.73442697054754147</v>
+        <v>0.73442700000000005</v>
       </c>
       <c r="C10">
-        <v>0.43089326601691869</v>
+        <v>0.43089300000000003</v>
       </c>
       <c r="D10">
-        <v>0.26557302945245848</v>
+        <v>0.265573</v>
       </c>
       <c r="E10">
-        <v>0.51326467738010706</v>
+        <v>0.51326499999999997</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -614,16 +614,16 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>0.26646585653765348</v>
+        <v>0.26646599999999998</v>
       </c>
       <c r="C11">
-        <v>9.2574095702099637E-2</v>
+        <v>9.2574000000000004E-2</v>
       </c>
       <c r="D11">
-        <v>0.73353414346234658</v>
+        <v>0.73353400000000002</v>
       </c>
       <c r="E11">
-        <v>0.2438881331580717</v>
+        <v>0.24388799999999999</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -631,16 +631,16 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>0.97574116926998178</v>
+        <v>0.97574099999999997</v>
       </c>
       <c r="C12">
-        <v>0.59137070201473951</v>
+        <v>0.59137099999999998</v>
       </c>
       <c r="D12">
-        <v>2.425883073001819E-2</v>
+        <v>2.4258999999999999E-2</v>
       </c>
       <c r="E12">
-        <v>0.61314511322512977</v>
+        <v>0.61314500000000005</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -648,16 +648,16 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>0.97268045571308859</v>
+        <v>0.97267999999999999</v>
       </c>
       <c r="C13">
-        <v>0.25399230778678339</v>
+        <v>0.253992</v>
       </c>
       <c r="D13">
-        <v>2.731954428691143E-2</v>
+        <v>2.7320000000000001E-2</v>
       </c>
       <c r="E13">
-        <v>0.77566700343625528</v>
+        <v>0.775667</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -665,16 +665,16 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>0.95421350137412986</v>
+        <v>0.95421400000000001</v>
       </c>
       <c r="C14">
-        <v>0.23350386457586131</v>
+        <v>0.23350399999999999</v>
       </c>
       <c r="D14">
-        <v>4.5786498625870121E-2</v>
+        <v>4.5786E-2</v>
       </c>
       <c r="E14">
-        <v>0.77357966097839104</v>
+        <v>0.77358000000000005</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -682,16 +682,16 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>0.91789933370329668</v>
+        <v>0.91789900000000002</v>
       </c>
       <c r="C15">
-        <v>0.2116059672908891</v>
+        <v>0.21160599999999999</v>
       </c>
       <c r="D15">
-        <v>8.2100666296703331E-2</v>
+        <v>8.2100999999999993E-2</v>
       </c>
       <c r="E15">
-        <v>0.7575889839463974</v>
+        <v>0.75758899999999996</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -699,16 +699,16 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>0.92734158082376328</v>
+        <v>0.927342</v>
       </c>
       <c r="C16">
-        <v>0.2180218071094901</v>
+        <v>0.21802199999999999</v>
       </c>
       <c r="D16">
-        <v>7.2658419176236708E-2</v>
+        <v>7.2658E-2</v>
       </c>
       <c r="E16">
-        <v>0.76135055662464257</v>
+        <v>0.761351</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -716,16 +716,16 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>0.92070394551549584</v>
+        <v>0.92070399999999997</v>
       </c>
       <c r="C17">
-        <v>0.1650309777155875</v>
+        <v>0.16503100000000001</v>
       </c>
       <c r="D17">
-        <v>7.9296054484504122E-2</v>
+        <v>7.9296000000000005E-2</v>
       </c>
       <c r="E17">
-        <v>0.79028280202542578</v>
+        <v>0.79028299999999996</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -733,52 +733,52 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>0.87576013872962644</v>
+        <v>0.87575999999999998</v>
       </c>
       <c r="C18">
-        <v>0.15987354648287669</v>
+        <v>0.15987399999999999</v>
       </c>
       <c r="D18">
-        <v>0.12423986127037349</v>
+        <v>0.12424</v>
       </c>
       <c r="E18">
-        <v>0.7550479458603252</v>
+        <v>0.75504800000000005</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B21" s="1">
         <f>AVERAGE(B1:B18)</f>
-        <v>0.86884516962673708</v>
+        <v>0.86884505555555558</v>
       </c>
       <c r="C21" s="1">
         <f t="shared" ref="C21:E21" si="0">AVERAGE(C1:C18)</f>
-        <v>0.31959983773901784</v>
+        <v>0.31959988888888891</v>
       </c>
       <c r="D21" s="1">
         <f t="shared" si="0"/>
-        <v>0.13115483037326292</v>
+        <v>0.13115494444444445</v>
       </c>
       <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>0.66169981139155809</v>
+        <v>0.66169994444444447</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B22" s="1">
         <f>STDEV(B1:B18)</f>
-        <v>0.16093780635595928</v>
+        <v>0.16093775295380558</v>
       </c>
       <c r="C22" s="1">
         <f t="shared" ref="C22:E22" si="1">STDEV(C1:C18)</f>
-        <v>0.15346780236223775</v>
+        <v>0.15346783116298102</v>
       </c>
       <c r="D22" s="1">
         <f t="shared" si="1"/>
-        <v>0.16093780635595903</v>
+        <v>0.16093775295380594</v>
       </c>
       <c r="E22" s="1">
         <f t="shared" si="1"/>
-        <v>0.13517928151325626</v>
+        <v>0.13517933710944816</v>
       </c>
     </row>
   </sheetData>

</xml_diff>